<commit_message>
Update Mini Project Product Backlog (2).xlsx
</commit_message>
<xml_diff>
--- a/Mini Project Product Backlog (2).xlsx
+++ b/Mini Project Product Backlog (2).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaanB\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ItsVa\Desktop\MiniProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB9B7BE-DB62-41C6-AEA7-C2103527B87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D2FB00-91FA-4B13-8200-B018C4883A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-360" yWindow="180" windowWidth="27030" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>If a player has taken damage in a fight he has to have the chance to use sertain health items he can find when completing quest or kill enemies</t>
+  </si>
+  <si>
+    <t>If the player has obtained several items he has to have an interface while viewing his items</t>
   </si>
 </sst>
 </file>
@@ -386,7 +389,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -818,7 +821,9 @@
       <c r="C10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3168,21 +3173,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010065DA0B4C524F55429CE2FD5B93B01F74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0b81802aa35bff97fe2d4068698eefb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea016a50-4395-487d-ae85-89d5607ff42b" xmlns:ns3="1f7ab50f-86ca-4990-8cf2-d29dc34c52f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b03203aba3005218e1fa3e02034dd03" ns2:_="" ns3:_="">
     <xsd:import namespace="ea016a50-4395-487d-ae85-89d5607ff42b"/>
@@ -3347,24 +3337,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C084766E-1400-4040-81BA-5DFB82754CBA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E847B739-67F9-4ADE-9E6F-0F08F6F51A70}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52455CA5-ED3E-453B-9081-F967EEE159E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3381,4 +3369,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E847B739-67F9-4ADE-9E6F-0F08F6F51A70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C084766E-1400-4040-81BA-5DFB82754CBA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>